<commit_message>
added some row's to the result table
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janco\OneDrive\Dokumente\Deep-Learning-Lab\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{18D43932-12DE-4F6A-A77B-F3EC850D1BD4}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7FB1A6C-49AD-4D28-8959-9142E3869449}"/>
   <bookViews>
     <workbookView xWindow="5454" yWindow="3366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Run</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>abs_rel</t>
   </si>
@@ -63,9 +60,6 @@
     <t>Ref. Paper</t>
   </si>
   <si>
-    <t>first run (no changes)</t>
-  </si>
-  <si>
     <t>Surface Normals 1</t>
   </si>
   <si>
@@ -73,6 +67,21 @@
   </si>
   <si>
     <t>first Run with our depth2normal.py code</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Run-Name (for the Log-file)</t>
+  </si>
+  <si>
+    <t>first run</t>
+  </si>
+  <si>
+    <t>no changes</t>
   </si>
 </sst>
 </file>
@@ -108,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -391,152 +401,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="E2">
+        <v>0.115</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.8630000000000004</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.193</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.877</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.871</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.192</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.878</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>32.395000000000003</v>
+      </c>
+      <c r="N3" s="1">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>0.115</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4.8630000000000004</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.193</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.877</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.95899999999999996</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.871</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4.82</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.192</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.878</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.95899999999999996</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>32.395000000000003</v>
-      </c>
-      <c r="L3" s="1">
-        <v>8.8999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>2.0289999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>92.852999999999994</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>31.963000000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>5.9550000000000001</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>0.13900000000000001</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>0.20499999999999999</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
         <v>450543.375</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>0.79800000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added first data into the result excel
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janco\OneDrive\Dokumente\Deep-Learning-Lab\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7FB1A6C-49AD-4D28-8959-9142E3869449}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91E5B348-01E9-4D88-AC23-338F6C438C3E}"/>
   <bookViews>
-    <workbookView xWindow="5454" yWindow="3366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29250" yWindow="4935" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>abs_rel</t>
   </si>
@@ -82,15 +82,150 @@
   </si>
   <si>
     <t>no changes</t>
+  </si>
+  <si>
+    <t>Loss Function</t>
+  </si>
+  <si>
+    <t>normals_04_02_20 (IN SEC Folder)</t>
+  </si>
+  <si>
+    <t>4ch_08_02_20</t>
+  </si>
+  <si>
+    <t>4ch_norm_05_02_20</t>
+  </si>
+  <si>
+    <t>4ch_continous_loss_08_02_20</t>
+  </si>
+  <si>
+    <t>4ch_binary_loss_8_2_20</t>
+  </si>
+  <si>
+    <t>4ch_norm_normal_loss</t>
+  </si>
+  <si>
+    <t>norm_pretrained_07_02_20</t>
+  </si>
+  <si>
+    <t>6ch_09_02_20</t>
+  </si>
+  <si>
+    <t>6ch_norm_09_02_20</t>
+  </si>
+  <si>
+    <t>rgb_binary_loss</t>
+  </si>
+  <si>
+    <t>rgb_norm_continous_8_2_20</t>
+  </si>
+  <si>
+    <t>Run-Time</t>
+  </si>
+  <si>
+    <t>Normals (Jun)</t>
+  </si>
+  <si>
+    <t>4 Channel</t>
+  </si>
+  <si>
+    <t>4 Ch + Normals</t>
+  </si>
+  <si>
+    <t>6 Ch</t>
+  </si>
+  <si>
+    <t>6 Ch + Normals</t>
+  </si>
+  <si>
+    <t>RGB + Normals</t>
+  </si>
+  <si>
+    <t>50h</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>17h</t>
+  </si>
+  <si>
+    <t>102: 23h fertig: Montag 11 Uhr</t>
+  </si>
+  <si>
+    <t>107: 55h fertig Montag 15 uhr</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>sup_continous</t>
+  </si>
+  <si>
+    <t>sup_binary</t>
+  </si>
+  <si>
+    <t>normal loss</t>
+  </si>
+  <si>
+    <t>sup + normals</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>104:</t>
+  </si>
+  <si>
+    <t>105:</t>
+  </si>
+  <si>
+    <t>101: 17h dertig: Montag 5 Uhr</t>
+  </si>
+  <si>
+    <t>4 Ch + norm + pretrained_encoder</t>
+  </si>
+  <si>
+    <t>first Run with our depth2normal.py code / evaluation with bugfixes by jun</t>
+  </si>
+  <si>
+    <t>Model-Name (Folder-Name)</t>
+  </si>
+  <si>
+    <t>normals_rgb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -105,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -113,14 +248,263 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -401,170 +785,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.20703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.68359375" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
+    <row r="3" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="29">
         <v>0.115</v>
       </c>
-      <c r="F2" s="1">
+      <c r="I3" s="29">
         <v>0.90300000000000002</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J3" s="29">
         <v>4.8630000000000004</v>
       </c>
-      <c r="H2" s="1">
+      <c r="K3" s="29">
         <v>0.193</v>
       </c>
-      <c r="I2" s="1">
+      <c r="L3" s="29">
         <v>0.877</v>
       </c>
-      <c r="J2" s="1">
+      <c r="M3" s="29">
         <v>0.95899999999999996</v>
       </c>
-      <c r="K2" s="1">
+      <c r="N3" s="29">
         <v>0.98099999999999998</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="30"/>
+    </row>
+    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="31">
         <v>0.114</v>
       </c>
-      <c r="F3" s="1">
+      <c r="I4" s="31">
         <v>0.871</v>
       </c>
-      <c r="G3" s="1">
+      <c r="J4" s="31">
         <v>4.82</v>
       </c>
-      <c r="H3" s="1">
+      <c r="K4" s="31">
         <v>0.192</v>
       </c>
-      <c r="I3" s="1">
+      <c r="L4" s="31">
         <v>0.878</v>
       </c>
-      <c r="J3" s="1">
+      <c r="M4" s="31">
         <v>0.95899999999999996</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N4" s="31">
         <v>0.98099999999999998</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31">
         <v>32.395000000000003</v>
       </c>
-      <c r="N3" s="1">
+      <c r="Q4" s="32">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2">
+    <row r="5" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
         <v>43851</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="31">
         <v>2.0289999999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="I5" s="31">
         <v>92.852999999999994</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J5" s="31">
         <v>31.963000000000001</v>
       </c>
-      <c r="H4" s="1">
+      <c r="K5" s="31">
         <v>5.9550000000000001</v>
       </c>
-      <c r="I4" s="1">
+      <c r="L5" s="31">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M5" s="31">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N5" s="31">
         <v>0.20499999999999999</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1">
+      <c r="O5" s="31"/>
+      <c r="P5" s="31">
         <v>450543.375</v>
       </c>
-      <c r="N4" s="1">
+      <c r="Q5" s="32">
         <v>0.79800000000000004</v>
       </c>
     </row>
+    <row r="6" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>43851</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="31">
+        <v>1.9730000000000001</v>
+      </c>
+      <c r="I6" s="31">
+        <v>87.905000000000001</v>
+      </c>
+      <c r="J6" s="31">
+        <v>29.31</v>
+      </c>
+      <c r="K6" s="31">
+        <v>1.589</v>
+      </c>
+      <c r="L6" s="31">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="M6" s="31">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="N6" s="31">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31">
+        <v>0.628</v>
+      </c>
+      <c r="Q6" s="32">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>43865</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="31">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="I7" s="31">
+        <v>23.484000000000002</v>
+      </c>
+      <c r="J7" s="31">
+        <v>17.556000000000001</v>
+      </c>
+      <c r="K7" s="31">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="L7" s="31">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M7" s="31">
+        <v>0.249</v>
+      </c>
+      <c r="N7" s="31">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>43866</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8" s="31">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="J8" s="31">
+        <v>5.7480000000000002</v>
+      </c>
+      <c r="K8" s="31">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="L8" s="31">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="M8" s="31">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="N8" s="31">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31">
+        <v>34.168999999999997</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>43866</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="H9" s="31">
+        <v>0.443</v>
+      </c>
+      <c r="I9" s="31">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="J9" s="31">
+        <v>12.083</v>
+      </c>
+      <c r="K9" s="31">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="L9" s="31">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M9" s="31">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="N9" s="31">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31">
+        <v>124.255</v>
+      </c>
+      <c r="Q9" s="32">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="31">
+        <v>0.443</v>
+      </c>
+      <c r="I10" s="31">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="J10" s="31">
+        <v>12.083</v>
+      </c>
+      <c r="K10" s="31">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="L10" s="31">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M10" s="31">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31">
+        <v>124.255</v>
+      </c>
+      <c r="Q10" s="32">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="32"/>
+    </row>
+    <row r="12" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+      <c r="A12" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="32"/>
+    </row>
+    <row r="13" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>43868</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="32"/>
+    </row>
+    <row r="14" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="27"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="32"/>
+    </row>
+    <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="32"/>
+    </row>
+    <row r="16" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="32"/>
+    </row>
+    <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="32"/>
+    </row>
+    <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>43869</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="32"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added actual results, but further investigations are necessary
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janco\OneDrive\Dokumente\Deep-Learning-Lab\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91E5B348-01E9-4D88-AC23-338F6C438C3E}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3293AE9-7834-4791-AE04-B43599293CC6}"/>
   <bookViews>
-    <workbookView xWindow="-29250" yWindow="4935" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4935" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>abs_rel</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>normals_rgb</t>
+  </si>
+  <si>
+    <t>muss neu ausgewertet werden, war noch wo anders gespeichert</t>
+  </si>
+  <si>
+    <t>not ready</t>
   </si>
 </sst>
 </file>
@@ -206,9 +212,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,13 +237,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -452,15 +470,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -468,12 +484,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -501,12 +511,24 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,659 +828,708 @@
     <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="11"/>
-    </row>
-    <row r="2" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32"/>
+    </row>
+    <row r="2" spans="1:18" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="29">
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="26">
         <v>0.115</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="26">
         <v>0.90300000000000002</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="26">
         <v>4.8630000000000004</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="26">
         <v>0.193</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="26">
         <v>0.877</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="26">
         <v>0.95899999999999996</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="26">
         <v>0.98099999999999998</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="30"/>
-    </row>
-    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20" t="s">
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="27"/>
+    </row>
+    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="31">
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="28">
         <v>0.114</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="28">
         <v>0.871</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="28">
         <v>4.82</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="28">
         <v>0.192</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="28">
         <v>0.878</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="28">
         <v>0.95899999999999996</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="28">
         <v>0.98099999999999998</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31">
+      <c r="O4" s="28"/>
+      <c r="P4" s="28">
         <v>32.395000000000003</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="29">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+    <row r="5" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
         <v>43851</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="31">
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="28">
         <v>2.0289999999999999</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="28">
         <v>92.852999999999994</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="28">
         <v>31.963000000000001</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="28">
         <v>5.9550000000000001</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="28">
         <v>0.13900000000000001</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="28">
         <v>0.20499999999999999</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31">
+      <c r="O5" s="28"/>
+      <c r="P5" s="28">
         <v>450543.375</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="29">
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+    <row r="6" spans="1:18" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
         <v>43851</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="31">
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="28">
         <v>1.9730000000000001</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="28">
         <v>87.905000000000001</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="28">
         <v>29.31</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="28">
         <v>1.589</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="28">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="28">
         <v>0.17399999999999999</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="28">
         <v>0.26400000000000001</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31">
+      <c r="O6" s="28"/>
+      <c r="P6" s="28">
         <v>0.628</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="29">
         <v>0.61199999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+    <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
         <v>43865</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="31">
+      <c r="G7" s="24"/>
+      <c r="H7" s="28">
         <v>0.95899999999999996</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="28">
         <v>23.484000000000002</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="28">
         <v>17.556000000000001</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="28">
         <v>2.2330000000000001</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="28">
         <v>0.13300000000000001</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="28">
         <v>0.249</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="28">
         <v>0.34599999999999997</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31">
+      <c r="O7" s="28"/>
+      <c r="P7" s="28">
         <v>0.14099999999999999</v>
       </c>
-      <c r="Q7" s="32">
+      <c r="Q7" s="29">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="R7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
         <v>43866</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="31">
+      <c r="G8" s="24"/>
+      <c r="H8" s="28">
         <v>0.14699999999999999</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="28">
         <v>1.4219999999999999</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="28">
         <v>5.7480000000000002</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="28">
         <v>0.22700000000000001</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="28">
         <v>0.82299999999999995</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="28">
         <v>0.93700000000000006</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="28">
         <v>0.97199999999999998</v>
       </c>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31">
+      <c r="O8" s="28"/>
+      <c r="P8" s="28">
         <v>34.168999999999997</v>
       </c>
-      <c r="Q8" s="32">
+      <c r="Q8" s="29">
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+    <row r="9" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
         <v>43866</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="31">
+      <c r="G9" s="24"/>
+      <c r="H9" s="33">
         <v>0.443</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="33">
         <v>4.7569999999999997</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="33">
         <v>12.083</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="33">
         <v>0.58799999999999997</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="33">
         <v>0.30299999999999999</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="33">
         <v>0.56100000000000005</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="33">
         <v>0.76600000000000001</v>
       </c>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31">
+      <c r="O9" s="33"/>
+      <c r="P9" s="33">
         <v>124.255</v>
       </c>
-      <c r="Q9" s="32">
+      <c r="Q9" s="34">
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+    <row r="10" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
         <v>43869</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="31">
+      <c r="G10" s="24"/>
+      <c r="H10" s="33">
         <v>0.443</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="33">
         <v>4.7569999999999997</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="33">
         <v>12.083</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="33">
         <v>0.58799999999999997</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="33">
         <v>0.30299999999999999</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="33">
         <v>0.56100000000000005</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="33">
         <v>0.76600000000000001</v>
       </c>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31">
+      <c r="O10" s="33"/>
+      <c r="P10" s="33">
         <v>124.255</v>
       </c>
-      <c r="Q10" s="32">
+      <c r="Q10" s="34">
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
         <v>43869</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="32"/>
-    </row>
-    <row r="12" spans="1:17" ht="75" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="G11" s="24"/>
+      <c r="H11" s="33">
+        <v>0.443</v>
+      </c>
+      <c r="I11" s="33">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="J11" s="33">
+        <v>12.083</v>
+      </c>
+      <c r="K11" s="33">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="L11" s="33">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M11" s="33">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="N11" s="33">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33">
+        <v>124.255</v>
+      </c>
+      <c r="Q11" s="34">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
         <v>43869</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="32"/>
-    </row>
-    <row r="13" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="G12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
         <v>43868</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="32"/>
-    </row>
-    <row r="14" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="33">
+        <v>0.443</v>
+      </c>
+      <c r="I13" s="33">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="J13" s="33">
+        <v>12.083</v>
+      </c>
+      <c r="K13" s="33">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="L13" s="33">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M13" s="33">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="N13" s="33">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33">
+        <v>124.255</v>
+      </c>
+      <c r="Q13" s="34">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="32"/>
-    </row>
-    <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+      <c r="G14" s="24"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29"/>
+    </row>
+    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
         <v>43869</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="32"/>
-    </row>
-    <row r="16" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="G15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
+    </row>
+    <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
         <v>43869</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="32"/>
+      <c r="G16" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="29"/>
     </row>
     <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+      <c r="A17" s="16">
         <v>43869</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="32"/>
+      <c r="G17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="29"/>
     </row>
     <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="A18" s="16">
         <v>43869</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="32"/>
+      <c r="G18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added Results to Endterm.pptx and Resluts excel
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janco\OneDrive\Dokumente\Deep-Learning-Lab\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{09BCD1F4-1A02-4B70-81FA-5E5C2948741F}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="13_ncr:1_{0E44B8B9-4900-47CB-835B-4C2B2A57D1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1812B03A-879C-4F96-ABAE-DF1B4A241B70}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>abs_rel</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>continous loss</t>
+  </si>
+  <si>
+    <t>4ch_norm_continous_loss_after_bugfix_10_02_20</t>
+  </si>
+  <si>
+    <t>rb_norm_cont_after_bugfix_10_02_20</t>
+  </si>
+  <si>
+    <t>3 Channel + Normal</t>
+  </si>
+  <si>
+    <t>15 h</t>
   </si>
 </sst>
 </file>
@@ -157,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +204,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -373,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -408,15 +432,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -699,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -724,16 +749,16 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="4" t="s">
@@ -869,7 +894,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -915,7 +940,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="19" t="s">
@@ -1091,41 +1116,97 @@
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
+    <row r="10" spans="1:16" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A10" s="14">
+        <v>43871</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>43</v>
+      </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="D10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="H10" s="24">
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="I10" s="24">
+        <v>5.484</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0.218</v>
+      </c>
+      <c r="K10" s="24">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="L10" s="24">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-    </row>
-    <row r="11" spans="1:16" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A11" s="14"/>
-      <c r="B11" s="18"/>
+      <c r="O10" s="24">
+        <v>39.795000000000002</v>
+      </c>
+      <c r="P10" s="24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A11" s="14">
+        <v>43871</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
+      <c r="D11" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0.443</v>
+      </c>
+      <c r="H11" s="24">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="I11" s="24">
+        <v>12.083</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="K11" s="24">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="M11" s="24">
+        <v>0.76600000000000001</v>
+      </c>
       <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="O11" s="24">
+        <v>0.125</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0.16400000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A12" s="14"/>

</xml_diff>